<commit_message>
Updated Mandarin Top Nav
Approved by Marlene
</commit_message>
<xml_diff>
--- a/assets/Mandarin Zones for Top Nav 2018.xlsx
+++ b/assets/Mandarin Zones for Top Nav 2018.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stuartridgway/Dropbox/Excella/VOA/Metrics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stuartridgway/Dropbox/Excella/VOA/Designs/IA/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59997484-68FF-A34E-915A-6FE5A514C83A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14160" xr2:uid="{39AFC7C5-DCEA-824A-B303-391336B17CC4}"/>
+    <workbookView xWindow="0" yWindow="940" windowWidth="25040" windowHeight="14160" xr2:uid="{39AFC7C5-DCEA-824A-B303-391336B17CC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Mandarin Zones for Top Nav - January 2018</t>
   </si>
@@ -77,95 +78,23 @@
     <t>military</t>
   </si>
   <si>
-    <t>教育</t>
-  </si>
-  <si>
-    <t>education</t>
-  </si>
-  <si>
-    <t>健康</t>
-  </si>
-  <si>
-    <t>health</t>
-  </si>
-  <si>
-    <t>专访</t>
-  </si>
-  <si>
-    <t>VOA-interviews</t>
-  </si>
-  <si>
-    <r>
-      <t>美中</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <charset val="134"/>
-      </rPr>
-      <t>关</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Microsoft JhengHei"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>系</t>
-    </r>
-  </si>
-  <si>
-    <t>us-china-relations-news</t>
-  </si>
-  <si>
-    <t>朝核问题</t>
-  </si>
-  <si>
-    <t>north-korea</t>
-  </si>
-  <si>
-    <r>
-      <t>两岸</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="SimSun"/>
-        <charset val="134"/>
-      </rPr>
-      <t>关</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Microsoft JhengHei"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>系</t>
-    </r>
-  </si>
-  <si>
-    <t>cross-strait-relations</t>
-  </si>
-  <si>
     <t>学英语</t>
   </si>
   <si>
     <t>learning-english</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>(link to Category Manager)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -197,8 +126,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="SimSun"/>
-      <charset val="134"/>
+      <name val="Microsoft JhengHei"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Microsoft JhengHei"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -221,11 +156,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,104 +487,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB981B4-DEC6-8942-989A-B3A3A1F6124C}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A3:C17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="7" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -652,70 +601,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="4" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>11</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>12</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>13</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>14</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>15</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>